<commit_message>
Limpeza e Explicação do Projeto
</commit_message>
<xml_diff>
--- a/Projeto_1/La Casa de Papel.xlsx
+++ b/Projeto_1/La Casa de Papel.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Desktop\INSPER\2° SEMESTRE\Ciência dos Dados\Projeto_1\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Desktop\INSPER\2° SEMESTRE\Ciência dos Dados\Projeto1CDados\Projeto_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3205DA58-A7E6-482B-9A00-24002E9DB960}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DCEB2F-28C4-4656-A7A8-36D708F2F5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -2043,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,7 +4471,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="A175" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Montagem do Classificador Naive-Bayes
</commit_message>
<xml_diff>
--- a/Projeto_1/La Casa de Papel.xlsx
+++ b/Projeto_1/La Casa de Papel.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Desktop\INSPER\2° SEMESTRE\Ciência dos Dados\Projeto1CDados\Projeto_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00DCEB2F-28C4-4656-A7A8-36D708F2F5E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE21BA-33E0-42ED-AFB5-5236C70C1FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Treinamento" sheetId="1" r:id="rId1"/>
@@ -2043,8 +2043,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B301"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A277" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A29" sqref="A29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4471,8 +4471,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView topLeftCell="A175" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B166" sqref="B166"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5798,7 +5798,7 @@
         <v>464</v>
       </c>
       <c r="B165">
-        <v>9</v>
+        <v>0</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Adição da Conclusão e explicação do classificador e laplace E adição de contextualização
</commit_message>
<xml_diff>
--- a/Projeto_1/La Casa de Papel.xlsx
+++ b/Projeto_1/La Casa de Papel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pedro Paulo\Desktop\INSPER\2° SEMESTRE\Ciência dos Dados\Projeto1CDados\Projeto_1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17CE21BA-33E0-42ED-AFB5-5236C70C1FB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FBAE408D-030E-4AE8-9208-CBFB826766A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="504" uniqueCount="502">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="505" uniqueCount="503">
   <si>
     <t>Treinamento</t>
   </si>
@@ -984,9 +984,6 @@
 eu quero: passar a tarde inteira deitada debaixo do ar condicionado vendo la casa de papel</t>
   </si>
   <si>
-    <t>Teste</t>
-  </si>
-  <si>
     <t>la casa de papel me decepcionou em um nível..</t>
   </si>
   <si>
@@ -1630,6 +1627,12 @@
   </si>
   <si>
     <t>Classificação</t>
+  </si>
+  <si>
+    <t>Teste</t>
+  </si>
+  <si>
+    <t>Chorei mto nessa série #SQN</t>
   </si>
 </sst>
 </file>
@@ -1696,13 +1699,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2058,7 +2062,7 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -4469,10 +4473,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:B201"/>
+  <dimension ref="A1:B203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A145" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B166" sqref="B166"/>
+    <sheetView tabSelected="1" topLeftCell="A187" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A203" sqref="A203"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4483,15 +4487,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>300</v>
+        <v>501</v>
       </c>
       <c r="B1" t="s">
-        <v>501</v>
+        <v>500</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -4499,7 +4503,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="B3">
         <v>0</v>
@@ -4507,7 +4511,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -4515,7 +4519,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B5">
         <v>0</v>
@@ -4523,7 +4527,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B6">
         <v>1</v>
@@ -4531,7 +4535,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B7">
         <v>1</v>
@@ -4539,7 +4543,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B8">
         <v>1</v>
@@ -4547,7 +4551,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
       <c r="B9">
         <v>0</v>
@@ -4555,7 +4559,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
       <c r="B10">
         <v>0</v>
@@ -4563,7 +4567,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B11">
         <v>1</v>
@@ -4571,7 +4575,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="B12">
         <v>0</v>
@@ -4579,7 +4583,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="B13">
         <v>0</v>
@@ -4587,7 +4591,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="B14">
         <v>0</v>
@@ -4595,7 +4599,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="B15">
         <v>0</v>
@@ -4603,7 +4607,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>315</v>
+        <v>314</v>
       </c>
       <c r="B16">
         <v>1</v>
@@ -4611,7 +4615,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="B17">
         <v>1</v>
@@ -4619,7 +4623,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="B18">
         <v>1</v>
@@ -4627,7 +4631,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="B19">
         <v>1</v>
@@ -4635,15 +4639,15 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>319</v>
-      </c>
-      <c r="B20">
-        <v>0</v>
+        <v>318</v>
+      </c>
+      <c r="B20" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>320</v>
+        <v>319</v>
       </c>
       <c r="B21">
         <v>0</v>
@@ -4651,7 +4655,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="B22">
         <v>0</v>
@@ -4659,7 +4663,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="B23">
         <v>0</v>
@@ -4667,7 +4671,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="B24">
         <v>0</v>
@@ -4675,7 +4679,7 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="B25">
         <v>0</v>
@@ -4683,7 +4687,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="B26" s="2">
         <v>1</v>
@@ -4691,7 +4695,7 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="B27">
         <v>0</v>
@@ -4699,7 +4703,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="B28">
         <v>0</v>
@@ -4707,7 +4711,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="B29">
         <v>1</v>
@@ -4715,7 +4719,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="B30">
         <v>0</v>
@@ -4723,7 +4727,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B31">
         <v>1</v>
@@ -4731,7 +4735,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B32">
         <v>1</v>
@@ -4739,7 +4743,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B33">
         <v>1</v>
@@ -4747,7 +4751,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="B34">
         <v>0</v>
@@ -4755,7 +4759,7 @@
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B35">
         <v>1</v>
@@ -4763,7 +4767,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="B36">
         <v>0</v>
@@ -4771,7 +4775,7 @@
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="B37">
         <v>0</v>
@@ -4779,7 +4783,7 @@
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="B38">
         <v>0</v>
@@ -4787,7 +4791,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="B39">
         <v>0</v>
@@ -4795,7 +4799,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="B40">
         <v>0</v>
@@ -4803,7 +4807,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="B41">
         <v>1</v>
@@ -4811,7 +4815,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B42">
         <v>0</v>
@@ -4819,7 +4823,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B43">
         <v>1</v>
@@ -4827,7 +4831,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B44">
         <v>0</v>
@@ -4835,7 +4839,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B45">
         <v>0</v>
@@ -4843,7 +4847,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="B46">
         <v>0</v>
@@ -4851,7 +4855,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="B47">
         <v>1</v>
@@ -4859,7 +4863,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="B48">
         <v>0</v>
@@ -4867,7 +4871,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="B49">
         <v>0</v>
@@ -4875,7 +4879,7 @@
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="B50">
         <v>1</v>
@@ -4883,7 +4887,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="B51">
         <v>1</v>
@@ -4891,7 +4895,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B52">
         <v>1</v>
@@ -4899,7 +4903,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B53">
         <v>1</v>
@@ -4907,7 +4911,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B54">
         <v>0</v>
@@ -4915,7 +4919,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B55">
         <v>0</v>
@@ -4923,7 +4927,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="B56">
         <v>0</v>
@@ -4931,7 +4935,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="B57">
         <v>0</v>
@@ -4939,7 +4943,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="B58">
         <v>1</v>
@@ -4947,7 +4951,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="B59">
         <v>0</v>
@@ -4955,7 +4959,7 @@
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="B60">
         <v>0</v>
@@ -4963,7 +4967,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="B61">
         <v>0</v>
@@ -4971,7 +4975,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="B62">
         <v>1</v>
@@ -4979,7 +4983,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="B63">
         <v>1</v>
@@ -4987,7 +4991,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="B64">
         <v>1</v>
@@ -4995,7 +4999,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="B65">
         <v>1</v>
@@ -5003,7 +5007,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="B66">
         <v>0</v>
@@ -5011,7 +5015,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="B67">
         <v>1</v>
@@ -5019,7 +5023,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="B68">
         <v>0</v>
@@ -5027,7 +5031,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="B69">
         <v>0</v>
@@ -5035,7 +5039,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="B70">
         <v>1</v>
@@ -5043,7 +5047,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="B71">
         <v>0</v>
@@ -5051,7 +5055,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B72">
         <v>1</v>
@@ -5059,7 +5063,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="B73">
         <v>1</v>
@@ -5067,7 +5071,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="B74">
         <v>1</v>
@@ -5075,7 +5079,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="B75">
         <v>1</v>
@@ -5083,7 +5087,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="B76">
         <v>0</v>
@@ -5091,7 +5095,7 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="B77">
         <v>1</v>
@@ -5099,7 +5103,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>377</v>
+        <v>376</v>
       </c>
       <c r="B78">
         <v>0</v>
@@ -5107,7 +5111,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>378</v>
+        <v>377</v>
       </c>
       <c r="B79">
         <v>0</v>
@@ -5115,7 +5119,7 @@
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="B80">
         <v>1</v>
@@ -5123,7 +5127,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="B81">
         <v>1</v>
@@ -5131,7 +5135,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="B82">
         <v>0</v>
@@ -5139,7 +5143,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="B83">
         <v>0</v>
@@ -5147,7 +5151,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="B84">
         <v>1</v>
@@ -5155,7 +5159,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="B85">
         <v>1</v>
@@ -5163,7 +5167,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="B86">
         <v>0</v>
@@ -5171,7 +5175,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="B87">
         <v>0</v>
@@ -5179,7 +5183,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="B88">
         <v>1</v>
@@ -5187,7 +5191,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B89">
         <v>1</v>
@@ -5195,7 +5199,7 @@
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="B90">
         <v>1</v>
@@ -5203,7 +5207,7 @@
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="B91">
         <v>0</v>
@@ -5211,7 +5215,7 @@
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="B92">
         <v>0</v>
@@ -5219,7 +5223,7 @@
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="B93">
         <v>0</v>
@@ -5227,7 +5231,7 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="B94">
         <v>1</v>
@@ -5235,7 +5239,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="B95">
         <v>1</v>
@@ -5243,7 +5247,7 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="B96">
         <v>0</v>
@@ -5251,7 +5255,7 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="B97">
         <v>0</v>
@@ -5259,7 +5263,7 @@
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="B98">
         <v>0</v>
@@ -5267,7 +5271,7 @@
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="B99">
         <v>1</v>
@@ -5275,7 +5279,7 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="B100">
         <v>1</v>
@@ -5283,7 +5287,7 @@
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="B101">
         <v>1</v>
@@ -5291,7 +5295,7 @@
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="B102">
         <v>1</v>
@@ -5299,7 +5303,7 @@
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B103">
         <v>0</v>
@@ -5307,7 +5311,7 @@
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B104">
         <v>1</v>
@@ -5315,7 +5319,7 @@
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B105">
         <v>0</v>
@@ -5323,7 +5327,7 @@
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B106">
         <v>0</v>
@@ -5331,7 +5335,7 @@
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B107">
         <v>0</v>
@@ -5339,7 +5343,7 @@
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B108">
         <v>1</v>
@@ -5347,7 +5351,7 @@
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="B109">
         <v>1</v>
@@ -5355,7 +5359,7 @@
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="B110">
         <v>1</v>
@@ -5363,7 +5367,7 @@
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="B111">
         <v>1</v>
@@ -5371,7 +5375,7 @@
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="B112">
         <v>0</v>
@@ -5379,7 +5383,7 @@
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="B113">
         <v>0</v>
@@ -5387,7 +5391,7 @@
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="B114">
         <v>0</v>
@@ -5395,7 +5399,7 @@
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="B115">
         <v>1</v>
@@ -5403,7 +5407,7 @@
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="B116">
         <v>1</v>
@@ -5411,7 +5415,7 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="B117">
         <v>0</v>
@@ -5419,7 +5423,7 @@
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="B118">
         <v>0</v>
@@ -5427,7 +5431,7 @@
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="B119">
         <v>1</v>
@@ -5435,7 +5439,7 @@
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="B120">
         <v>0</v>
@@ -5443,7 +5447,7 @@
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="B121">
         <v>1</v>
@@ -5451,7 +5455,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="B122">
         <v>0</v>
@@ -5459,7 +5463,7 @@
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
       <c r="B123">
         <v>0</v>
@@ -5467,7 +5471,7 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>423</v>
+        <v>422</v>
       </c>
       <c r="B124">
         <v>1</v>
@@ -5475,7 +5479,7 @@
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>424</v>
+        <v>423</v>
       </c>
       <c r="B125">
         <v>1</v>
@@ -5483,7 +5487,7 @@
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>425</v>
+        <v>424</v>
       </c>
       <c r="B126">
         <v>1</v>
@@ -5491,7 +5495,7 @@
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>426</v>
+        <v>425</v>
       </c>
       <c r="B127">
         <v>0</v>
@@ -5499,7 +5503,7 @@
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="B128">
         <v>1</v>
@@ -5507,7 +5511,7 @@
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="B129">
         <v>1</v>
@@ -5515,7 +5519,7 @@
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>429</v>
+        <v>428</v>
       </c>
       <c r="B130">
         <v>0</v>
@@ -5523,7 +5527,7 @@
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>430</v>
+        <v>429</v>
       </c>
       <c r="B131">
         <v>0</v>
@@ -5531,7 +5535,7 @@
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>431</v>
+        <v>430</v>
       </c>
       <c r="B132">
         <v>0</v>
@@ -5539,7 +5543,7 @@
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>432</v>
+        <v>431</v>
       </c>
       <c r="B133">
         <v>1</v>
@@ -5547,7 +5551,7 @@
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>433</v>
+        <v>432</v>
       </c>
       <c r="B134">
         <v>0</v>
@@ -5555,7 +5559,7 @@
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>434</v>
+        <v>433</v>
       </c>
       <c r="B135">
         <v>0</v>
@@ -5563,7 +5567,7 @@
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="B136">
         <v>0</v>
@@ -5571,7 +5575,7 @@
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>436</v>
+        <v>435</v>
       </c>
       <c r="B137">
         <v>1</v>
@@ -5579,7 +5583,7 @@
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>437</v>
+        <v>436</v>
       </c>
       <c r="B138">
         <v>0</v>
@@ -5587,7 +5591,7 @@
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>438</v>
+        <v>437</v>
       </c>
       <c r="B139">
         <v>1</v>
@@ -5595,7 +5599,7 @@
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>439</v>
+        <v>438</v>
       </c>
       <c r="B140">
         <v>0</v>
@@ -5603,7 +5607,7 @@
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>440</v>
+        <v>439</v>
       </c>
       <c r="B141">
         <v>0</v>
@@ -5611,7 +5615,7 @@
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>441</v>
+        <v>440</v>
       </c>
       <c r="B142">
         <v>0</v>
@@ -5619,7 +5623,7 @@
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="B143">
         <v>0</v>
@@ -5627,7 +5631,7 @@
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="B144">
         <v>1</v>
@@ -5635,7 +5639,7 @@
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>444</v>
+        <v>443</v>
       </c>
       <c r="B145">
         <v>1</v>
@@ -5643,7 +5647,7 @@
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>445</v>
+        <v>444</v>
       </c>
       <c r="B146">
         <v>1</v>
@@ -5651,7 +5655,7 @@
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>446</v>
+        <v>445</v>
       </c>
       <c r="B147">
         <v>0</v>
@@ -5659,7 +5663,7 @@
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="B148">
         <v>1</v>
@@ -5667,7 +5671,7 @@
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>448</v>
+        <v>447</v>
       </c>
       <c r="B149">
         <v>1</v>
@@ -5675,7 +5679,7 @@
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>449</v>
+        <v>448</v>
       </c>
       <c r="B150">
         <v>1</v>
@@ -5683,7 +5687,7 @@
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>450</v>
+        <v>449</v>
       </c>
       <c r="B151">
         <v>0</v>
@@ -5691,7 +5695,7 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>451</v>
+        <v>450</v>
       </c>
       <c r="B152">
         <v>0</v>
@@ -5699,7 +5703,7 @@
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
       <c r="B153">
         <v>0</v>
@@ -5707,7 +5711,7 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>453</v>
+        <v>452</v>
       </c>
       <c r="B154">
         <v>0</v>
@@ -5715,7 +5719,7 @@
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>454</v>
+        <v>453</v>
       </c>
       <c r="B155">
         <v>1</v>
@@ -5723,7 +5727,7 @@
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="B156">
         <v>0</v>
@@ -5731,7 +5735,7 @@
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>456</v>
+        <v>455</v>
       </c>
       <c r="B157">
         <v>1</v>
@@ -5739,7 +5743,7 @@
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="B158">
         <v>0</v>
@@ -5747,7 +5751,7 @@
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="B159">
         <v>0</v>
@@ -5755,7 +5759,7 @@
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="B160">
         <v>0</v>
@@ -5763,7 +5767,7 @@
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="B161">
         <v>0</v>
@@ -5771,7 +5775,7 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="B162">
         <v>0</v>
@@ -5779,7 +5783,7 @@
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
       <c r="B163">
         <v>0</v>
@@ -5787,7 +5791,7 @@
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
       <c r="B164">
         <v>1</v>
@@ -5795,7 +5799,7 @@
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="B165">
         <v>0</v>
@@ -5803,7 +5807,7 @@
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="B166">
         <v>1</v>
@@ -5811,7 +5815,7 @@
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
       <c r="B167">
         <v>1</v>
@@ -5819,7 +5823,7 @@
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>467</v>
+        <v>466</v>
       </c>
       <c r="B168">
         <v>0</v>
@@ -5827,7 +5831,7 @@
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>468</v>
+        <v>467</v>
       </c>
       <c r="B169">
         <v>0</v>
@@ -5835,7 +5839,7 @@
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>469</v>
+        <v>468</v>
       </c>
       <c r="B170">
         <v>1</v>
@@ -5843,7 +5847,7 @@
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>470</v>
+        <v>469</v>
       </c>
       <c r="B171">
         <v>1</v>
@@ -5851,7 +5855,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
       <c r="B172">
         <v>0</v>
@@ -5859,7 +5863,7 @@
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="B173">
         <v>0</v>
@@ -5867,7 +5871,7 @@
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
       <c r="B174">
         <v>0</v>
@@ -5875,7 +5879,7 @@
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
       <c r="B175">
         <v>1</v>
@@ -5883,7 +5887,7 @@
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>475</v>
+        <v>474</v>
       </c>
       <c r="B176">
         <v>0</v>
@@ -5891,7 +5895,7 @@
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="B177">
         <v>0</v>
@@ -5899,7 +5903,7 @@
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A178" t="s">
-        <v>477</v>
+        <v>476</v>
       </c>
       <c r="B178">
         <v>0</v>
@@ -5907,7 +5911,7 @@
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A179" t="s">
-        <v>478</v>
+        <v>477</v>
       </c>
       <c r="B179">
         <v>0</v>
@@ -5915,7 +5919,7 @@
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A180" t="s">
-        <v>479</v>
+        <v>478</v>
       </c>
       <c r="B180">
         <v>0</v>
@@ -5923,7 +5927,7 @@
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A181" t="s">
-        <v>480</v>
+        <v>479</v>
       </c>
       <c r="B181">
         <v>0</v>
@@ -5931,7 +5935,7 @@
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A182" t="s">
-        <v>481</v>
+        <v>480</v>
       </c>
       <c r="B182">
         <v>0</v>
@@ -5939,7 +5943,7 @@
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A183" t="s">
-        <v>482</v>
+        <v>481</v>
       </c>
       <c r="B183">
         <v>1</v>
@@ -5947,7 +5951,7 @@
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A184" t="s">
-        <v>483</v>
+        <v>482</v>
       </c>
       <c r="B184">
         <v>0</v>
@@ -5955,7 +5959,7 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A185" t="s">
-        <v>484</v>
+        <v>483</v>
       </c>
       <c r="B185">
         <v>1</v>
@@ -5963,7 +5967,7 @@
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A186" t="s">
-        <v>485</v>
+        <v>484</v>
       </c>
       <c r="B186">
         <v>1</v>
@@ -5971,7 +5975,7 @@
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A187" t="s">
-        <v>486</v>
+        <v>485</v>
       </c>
       <c r="B187">
         <v>0</v>
@@ -5979,7 +5983,7 @@
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A188" t="s">
-        <v>487</v>
+        <v>486</v>
       </c>
       <c r="B188">
         <v>0</v>
@@ -5987,7 +5991,7 @@
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A189" t="s">
-        <v>488</v>
+        <v>487</v>
       </c>
       <c r="B189">
         <v>1</v>
@@ -5995,7 +5999,7 @@
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A190" t="s">
-        <v>489</v>
+        <v>488</v>
       </c>
       <c r="B190">
         <v>0</v>
@@ -6003,7 +6007,7 @@
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A191" t="s">
-        <v>490</v>
+        <v>489</v>
       </c>
       <c r="B191">
         <v>0</v>
@@ -6011,7 +6015,7 @@
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A192" t="s">
-        <v>491</v>
+        <v>490</v>
       </c>
       <c r="B192">
         <v>0</v>
@@ -6019,7 +6023,7 @@
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A193" t="s">
-        <v>492</v>
+        <v>491</v>
       </c>
       <c r="B193">
         <v>1</v>
@@ -6027,7 +6031,7 @@
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A194" t="s">
-        <v>493</v>
+        <v>492</v>
       </c>
       <c r="B194">
         <v>0</v>
@@ -6035,7 +6039,7 @@
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A195" t="s">
-        <v>494</v>
+        <v>493</v>
       </c>
       <c r="B195">
         <v>1</v>
@@ -6043,7 +6047,7 @@
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A196" t="s">
-        <v>495</v>
+        <v>494</v>
       </c>
       <c r="B196">
         <v>0</v>
@@ -6051,7 +6055,7 @@
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A197" t="s">
-        <v>496</v>
+        <v>495</v>
       </c>
       <c r="B197">
         <v>1</v>
@@ -6059,7 +6063,7 @@
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A198" t="s">
-        <v>497</v>
+        <v>496</v>
       </c>
       <c r="B198">
         <v>0</v>
@@ -6067,7 +6071,7 @@
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A199" t="s">
-        <v>498</v>
+        <v>497</v>
       </c>
       <c r="B199">
         <v>1</v>
@@ -6075,7 +6079,7 @@
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A200" t="s">
-        <v>499</v>
+        <v>498</v>
       </c>
       <c r="B200">
         <v>0</v>
@@ -6083,13 +6087,23 @@
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A201" t="s">
-        <v>500</v>
+        <v>499</v>
       </c>
       <c r="B201">
         <v>1</v>
       </c>
+    </row>
+    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A202" t="s">
+        <v>502</v>
+      </c>
+    </row>
+    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A203" s="3"/>
+      <c r="B203" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>